<commit_message>
Submit Test design 5
</commit_message>
<xml_diff>
--- a/Assignment5/TestDesign/TestDesign-Assignment5-QuynhAnh.xlsx
+++ b/Assignment5/TestDesign/TestDesign-Assignment5-QuynhAnh.xlsx
@@ -2753,9 +2753,6 @@
     <t>Delete button is clickable</t>
   </si>
   <si>
-    <t xml:space="preserve">Check dispslaying Confirmation pop-up </t>
-  </si>
-  <si>
     <t>- Confirmation pop-up is displayed
 - Confirmation pop-up contains:
 + Alert: "Are you sure you want to delete this address?"
@@ -2796,6 +2793,9 @@
   </si>
   <si>
     <t>Check function when click on Save button in the Edit My Address screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check displaying Confirmation pop-up </t>
   </si>
 </sst>
 </file>
@@ -4325,23 +4325,53 @@
     <xf numFmtId="0" fontId="64" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="16" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="5" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="64" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="5" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="16" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4349,26 +4379,44 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="30" fillId="3" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="18" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="20" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="15" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="16" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="11" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="46" fillId="0" borderId="6" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="15" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4376,6 +4424,15 @@
     <xf numFmtId="0" fontId="48" fillId="0" borderId="11" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="6" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="15" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="11" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="166" fontId="43" fillId="12" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -4385,68 +4442,11 @@
     <xf numFmtId="166" fontId="44" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="30" fillId="3" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="166" fontId="3" fillId="2" borderId="8" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="3" fillId="2" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="15" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="11" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="6" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="15" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="11" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="46" fillId="0" borderId="6" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="18" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="20" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="16" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="16" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="27">
@@ -6243,8 +6243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -6259,10 +6259,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="1" customFormat="1" ht="14.25">
-      <c r="A1" s="193"/>
-      <c r="B1" s="193"/>
-      <c r="C1" s="193"/>
-      <c r="D1" s="193"/>
+      <c r="A1" s="201"/>
+      <c r="B1" s="201"/>
+      <c r="C1" s="201"/>
+      <c r="D1" s="201"/>
       <c r="E1" s="34"/>
       <c r="F1" s="34"/>
       <c r="G1" s="34"/>
@@ -6271,13 +6271,13 @@
       <c r="J1" s="34"/>
     </row>
     <row r="2" spans="1:24" s="1" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A2" s="194" t="s">
+      <c r="A2" s="202" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="194"/>
-      <c r="C2" s="194"/>
-      <c r="D2" s="194"/>
-      <c r="E2" s="202"/>
+      <c r="B2" s="202"/>
+      <c r="C2" s="202"/>
+      <c r="D2" s="202"/>
+      <c r="E2" s="197"/>
       <c r="F2" s="23"/>
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
@@ -6286,9 +6286,9 @@
     </row>
     <row r="3" spans="1:24" s="1" customFormat="1" ht="31.5" customHeight="1">
       <c r="A3" s="47"/>
-      <c r="C3" s="203"/>
-      <c r="D3" s="203"/>
-      <c r="E3" s="202"/>
+      <c r="C3" s="198"/>
+      <c r="D3" s="198"/>
+      <c r="E3" s="197"/>
       <c r="F3" s="23"/>
       <c r="G3" s="23"/>
       <c r="H3" s="23"/>
@@ -6299,11 +6299,11 @@
       <c r="A4" s="139" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="196" t="s">
+      <c r="B4" s="199" t="s">
         <v>418</v>
       </c>
-      <c r="C4" s="196"/>
-      <c r="D4" s="196"/>
+      <c r="C4" s="199"/>
+      <c r="D4" s="199"/>
       <c r="E4" s="39"/>
       <c r="F4" s="39"/>
       <c r="G4" s="39"/>
@@ -6317,11 +6317,11 @@
       <c r="A5" s="139" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="195" t="s">
+      <c r="B5" s="200" t="s">
         <v>422</v>
       </c>
-      <c r="C5" s="196"/>
-      <c r="D5" s="196"/>
+      <c r="C5" s="199"/>
+      <c r="D5" s="199"/>
       <c r="E5" s="39"/>
       <c r="F5" s="39"/>
       <c r="G5" s="39"/>
@@ -6335,11 +6335,11 @@
       <c r="A6" s="139" t="s">
         <v>96</v>
       </c>
-      <c r="B6" s="195" t="s">
+      <c r="B6" s="200" t="s">
         <v>421</v>
       </c>
-      <c r="C6" s="196"/>
-      <c r="D6" s="196"/>
+      <c r="C6" s="199"/>
+      <c r="D6" s="199"/>
       <c r="E6" s="39"/>
       <c r="F6" s="39"/>
       <c r="G6" s="39"/>
@@ -6350,9 +6350,9 @@
       <c r="A7" s="139" t="s">
         <v>98</v>
       </c>
-      <c r="B7" s="196"/>
-      <c r="C7" s="196"/>
-      <c r="D7" s="196"/>
+      <c r="B7" s="199"/>
+      <c r="C7" s="199"/>
+      <c r="D7" s="199"/>
       <c r="E7" s="39"/>
       <c r="F7" s="39"/>
       <c r="G7" s="39"/>
@@ -6364,9 +6364,9 @@
       <c r="A8" s="139" t="s">
         <v>100</v>
       </c>
-      <c r="B8" s="197"/>
-      <c r="C8" s="197"/>
-      <c r="D8" s="197"/>
+      <c r="B8" s="203"/>
+      <c r="C8" s="203"/>
+      <c r="D8" s="203"/>
       <c r="E8" s="39"/>
     </row>
     <row r="9" spans="1:24" s="43" customFormat="1">
@@ -6509,11 +6509,11 @@
       <c r="C16" s="50"/>
       <c r="D16" s="51"/>
       <c r="E16" s="56"/>
-      <c r="F16" s="198" t="s">
+      <c r="F16" s="193" t="s">
         <v>101</v>
       </c>
-      <c r="G16" s="198"/>
-      <c r="H16" s="198"/>
+      <c r="G16" s="193"/>
+      <c r="H16" s="193"/>
       <c r="I16" s="57"/>
     </row>
     <row r="17" spans="1:9" s="44" customFormat="1" ht="38.25">
@@ -6547,11 +6547,11 @@
     </row>
     <row r="18" spans="1:9" s="44" customFormat="1" ht="15.75" customHeight="1">
       <c r="A18" s="67"/>
-      <c r="B18" s="231" t="s">
+      <c r="B18" s="194" t="s">
         <v>419</v>
       </c>
-      <c r="C18" s="232"/>
-      <c r="D18" s="233"/>
+      <c r="C18" s="195"/>
+      <c r="D18" s="196"/>
       <c r="E18" s="67"/>
       <c r="F18" s="68"/>
       <c r="G18" s="68"/>
@@ -6560,11 +6560,11 @@
     </row>
     <row r="19" spans="1:9" s="44" customFormat="1" ht="15.75" customHeight="1">
       <c r="A19" s="67"/>
-      <c r="B19" s="231" t="s">
+      <c r="B19" s="194" t="s">
         <v>420</v>
       </c>
-      <c r="C19" s="232"/>
-      <c r="D19" s="233"/>
+      <c r="C19" s="195"/>
+      <c r="D19" s="196"/>
       <c r="E19" s="67"/>
       <c r="F19" s="68"/>
       <c r="G19" s="68"/>
@@ -6576,10 +6576,10 @@
         <v>1</v>
       </c>
       <c r="B20" s="52" t="s">
+        <v>426</v>
+      </c>
+      <c r="C20" s="52" t="s">
         <v>427</v>
-      </c>
-      <c r="C20" s="52" t="s">
-        <v>428</v>
       </c>
       <c r="D20" s="53" t="s">
         <v>423</v>
@@ -6592,17 +6592,17 @@
     </row>
     <row r="21" spans="1:9" s="45" customFormat="1" ht="102">
       <c r="A21" s="58">
-        <f ca="1">IF(OFFSET(A21,-1,0) ="",OFFSET(A21,-2,0)+1,OFFSET(A21,-1,0)+1 )</f>
+        <f t="shared" ref="A21:A26" ca="1" si="0">IF(OFFSET(A21,-1,0) ="",OFFSET(A21,-2,0)+1,OFFSET(A21,-1,0)+1 )</f>
         <v>2</v>
       </c>
       <c r="B21" s="52" t="s">
+        <v>435</v>
+      </c>
+      <c r="C21" s="52" t="s">
+        <v>428</v>
+      </c>
+      <c r="D21" s="53" t="s">
         <v>424</v>
-      </c>
-      <c r="C21" s="52" t="s">
-        <v>429</v>
-      </c>
-      <c r="D21" s="53" t="s">
-        <v>425</v>
       </c>
       <c r="E21" s="54"/>
       <c r="F21" s="52"/>
@@ -6612,17 +6612,17 @@
     </row>
     <row r="22" spans="1:9" s="45" customFormat="1" ht="89.25">
       <c r="A22" s="58">
-        <f ca="1">IF(OFFSET(A22,-1,0) ="",OFFSET(A22,-2,0)+1,OFFSET(A22,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
       <c r="B22" s="52" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C22" s="52" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D22" s="60" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E22" s="52"/>
       <c r="F22" s="52"/>
@@ -6632,11 +6632,11 @@
     </row>
     <row r="23" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A23" s="58">
-        <f ca="1">IF(OFFSET(A23,-1,0) ="",OFFSET(A23,-2,0)+1,OFFSET(A23,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="0"/>
         <v>4</v>
       </c>
       <c r="B23" s="52" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C23" s="52"/>
       <c r="D23" s="54"/>
@@ -6648,11 +6648,11 @@
     </row>
     <row r="24" spans="1:9" s="48" customFormat="1" ht="25.5">
       <c r="A24" s="58">
-        <f ca="1">IF(OFFSET(A24,-1,0) ="",OFFSET(A24,-2,0)+1,OFFSET(A24,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
       <c r="B24" s="52" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C24" s="52"/>
       <c r="D24" s="54"/>
@@ -6664,11 +6664,11 @@
     </row>
     <row r="25" spans="1:9" s="48" customFormat="1" ht="25.5">
       <c r="A25" s="58">
-        <f ca="1">IF(OFFSET(A25,-1,0) ="",OFFSET(A25,-2,0)+1,OFFSET(A25,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="0"/>
         <v>6</v>
       </c>
       <c r="B25" s="52" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C25" s="52"/>
       <c r="D25" s="54"/>
@@ -6680,11 +6680,11 @@
     </row>
     <row r="26" spans="1:9" s="48" customFormat="1" ht="25.5">
       <c r="A26" s="58">
-        <f ca="1">IF(OFFSET(A26,-1,0) ="",OFFSET(A26,-2,0)+1,OFFSET(A26,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="0"/>
         <v>7</v>
       </c>
       <c r="B26" s="52" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C26" s="52"/>
       <c r="D26" s="60"/>
@@ -6695,10 +6695,7 @@
       <c r="I26" s="61"/>
     </row>
     <row r="27" spans="1:9" s="48" customFormat="1" ht="14.25">
-      <c r="A27" s="58">
-        <f t="shared" ref="A27:A29" ca="1" si="0">IF(OFFSET(A27,-1,0) ="",OFFSET(A27,-2,0)+1,OFFSET(A27,-1,0)+1 )</f>
-        <v>8</v>
-      </c>
+      <c r="A27" s="58"/>
       <c r="B27" s="52"/>
       <c r="C27" s="52"/>
       <c r="D27" s="54"/>
@@ -6709,10 +6706,7 @@
       <c r="I27" s="61"/>
     </row>
     <row r="28" spans="1:9" s="48" customFormat="1" ht="14.25">
-      <c r="A28" s="58">
-        <f t="shared" ca="1" si="0"/>
-        <v>9</v>
-      </c>
+      <c r="A28" s="58"/>
       <c r="B28" s="52"/>
       <c r="C28" s="52"/>
       <c r="D28" s="54"/>
@@ -6723,10 +6717,7 @@
       <c r="I28" s="61"/>
     </row>
     <row r="29" spans="1:9" s="48" customFormat="1" ht="14.25">
-      <c r="A29" s="58">
-        <f t="shared" ca="1" si="0"/>
-        <v>10</v>
-      </c>
+      <c r="A29" s="58"/>
       <c r="B29" s="52"/>
       <c r="C29" s="52"/>
       <c r="D29" s="54"/>
@@ -6737,10 +6728,7 @@
       <c r="I29" s="61"/>
     </row>
     <row r="30" spans="1:9" s="48" customFormat="1" ht="14.25">
-      <c r="A30" s="62">
-        <f t="shared" ref="A30:A50" ca="1" si="1">IF(OFFSET(A30,-1,0) ="",OFFSET(A30,-2,0)+1,OFFSET(A30,-1,0)+1 )</f>
-        <v>11</v>
-      </c>
+      <c r="A30" s="62"/>
       <c r="B30" s="52"/>
       <c r="C30" s="52"/>
       <c r="D30" s="54"/>
@@ -6751,10 +6739,7 @@
       <c r="I30" s="62"/>
     </row>
     <row r="31" spans="1:9" s="48" customFormat="1" ht="14.25">
-      <c r="A31" s="62">
-        <f t="shared" ca="1" si="1"/>
-        <v>12</v>
-      </c>
+      <c r="A31" s="62"/>
       <c r="B31" s="52"/>
       <c r="C31" s="52"/>
       <c r="D31" s="54"/>
@@ -6765,10 +6750,7 @@
       <c r="I31" s="62"/>
     </row>
     <row r="32" spans="1:9" s="48" customFormat="1" ht="14.25">
-      <c r="A32" s="62">
-        <f t="shared" ca="1" si="1"/>
-        <v>13</v>
-      </c>
+      <c r="A32" s="62"/>
       <c r="B32" s="52"/>
       <c r="C32" s="52"/>
       <c r="D32" s="54"/>
@@ -6779,10 +6761,7 @@
       <c r="I32" s="62"/>
     </row>
     <row r="33" spans="1:9" s="48" customFormat="1" ht="14.25">
-      <c r="A33" s="62">
-        <f t="shared" ca="1" si="1"/>
-        <v>14</v>
-      </c>
+      <c r="A33" s="62"/>
       <c r="B33" s="52"/>
       <c r="C33" s="52"/>
       <c r="D33" s="60"/>
@@ -6793,10 +6772,7 @@
       <c r="I33" s="62"/>
     </row>
     <row r="34" spans="1:9" s="48" customFormat="1" ht="14.25">
-      <c r="A34" s="62">
-        <f t="shared" ca="1" si="1"/>
-        <v>15</v>
-      </c>
+      <c r="A34" s="62"/>
       <c r="B34" s="52"/>
       <c r="C34" s="52"/>
       <c r="D34" s="60"/>
@@ -6807,10 +6783,7 @@
       <c r="I34" s="62"/>
     </row>
     <row r="35" spans="1:9" s="48" customFormat="1" ht="14.25">
-      <c r="A35" s="62">
-        <f t="shared" ca="1" si="1"/>
-        <v>16</v>
-      </c>
+      <c r="A35" s="62"/>
       <c r="B35" s="52"/>
       <c r="C35" s="52"/>
       <c r="D35" s="60"/>
@@ -6821,10 +6794,7 @@
       <c r="I35" s="62"/>
     </row>
     <row r="36" spans="1:9" s="48" customFormat="1" ht="14.25">
-      <c r="A36" s="62">
-        <f t="shared" ca="1" si="1"/>
-        <v>17</v>
-      </c>
+      <c r="A36" s="62"/>
       <c r="B36" s="52"/>
       <c r="C36" s="52"/>
       <c r="D36" s="54"/>
@@ -6835,10 +6805,7 @@
       <c r="I36" s="62"/>
     </row>
     <row r="37" spans="1:9" s="48" customFormat="1" ht="14.25">
-      <c r="A37" s="62">
-        <f t="shared" ca="1" si="1"/>
-        <v>18</v>
-      </c>
+      <c r="A37" s="62"/>
       <c r="B37" s="52"/>
       <c r="C37" s="52"/>
       <c r="D37" s="54"/>
@@ -6849,10 +6816,7 @@
       <c r="I37" s="62"/>
     </row>
     <row r="38" spans="1:9" s="48" customFormat="1" ht="14.25">
-      <c r="A38" s="62">
-        <f t="shared" ca="1" si="1"/>
-        <v>19</v>
-      </c>
+      <c r="A38" s="62"/>
       <c r="B38" s="52"/>
       <c r="C38" s="52"/>
       <c r="D38" s="53"/>
@@ -6863,10 +6827,7 @@
       <c r="I38" s="62"/>
     </row>
     <row r="39" spans="1:9" s="48" customFormat="1" ht="14.25">
-      <c r="A39" s="62">
-        <f t="shared" ca="1" si="1"/>
-        <v>20</v>
-      </c>
+      <c r="A39" s="62"/>
       <c r="B39" s="52"/>
       <c r="C39" s="52"/>
       <c r="D39" s="60"/>
@@ -6877,10 +6838,7 @@
       <c r="I39" s="62"/>
     </row>
     <row r="40" spans="1:9" s="48" customFormat="1" ht="14.25">
-      <c r="A40" s="62">
-        <f t="shared" ca="1" si="1"/>
-        <v>21</v>
-      </c>
+      <c r="A40" s="62"/>
       <c r="B40" s="52"/>
       <c r="C40" s="52"/>
       <c r="D40" s="60"/>
@@ -6891,10 +6849,7 @@
       <c r="I40" s="62"/>
     </row>
     <row r="41" spans="1:9" s="48" customFormat="1" ht="14.25">
-      <c r="A41" s="62">
-        <f t="shared" ca="1" si="1"/>
-        <v>22</v>
-      </c>
+      <c r="A41" s="62"/>
       <c r="B41" s="52"/>
       <c r="C41" s="52"/>
       <c r="D41" s="54"/>
@@ -6905,10 +6860,7 @@
       <c r="I41" s="62"/>
     </row>
     <row r="42" spans="1:9" s="48" customFormat="1" ht="14.25">
-      <c r="A42" s="62">
-        <f t="shared" ca="1" si="1"/>
-        <v>23</v>
-      </c>
+      <c r="A42" s="62"/>
       <c r="B42" s="52"/>
       <c r="C42" s="52"/>
       <c r="D42" s="54"/>
@@ -6919,10 +6871,7 @@
       <c r="I42" s="62"/>
     </row>
     <row r="43" spans="1:9" s="48" customFormat="1" ht="14.25">
-      <c r="A43" s="62">
-        <f t="shared" ca="1" si="1"/>
-        <v>24</v>
-      </c>
+      <c r="A43" s="62"/>
       <c r="B43" s="52"/>
       <c r="C43" s="52"/>
       <c r="D43" s="54"/>
@@ -6933,10 +6882,7 @@
       <c r="I43" s="62"/>
     </row>
     <row r="44" spans="1:9" s="48" customFormat="1" ht="14.25">
-      <c r="A44" s="62">
-        <f t="shared" ca="1" si="1"/>
-        <v>25</v>
-      </c>
+      <c r="A44" s="62"/>
       <c r="B44" s="52"/>
       <c r="C44" s="52"/>
       <c r="D44" s="54"/>
@@ -6947,10 +6893,7 @@
       <c r="I44" s="62"/>
     </row>
     <row r="45" spans="1:9" s="48" customFormat="1" ht="14.25">
-      <c r="A45" s="62">
-        <f t="shared" ca="1" si="1"/>
-        <v>26</v>
-      </c>
+      <c r="A45" s="62"/>
       <c r="B45" s="52"/>
       <c r="C45" s="52"/>
       <c r="D45" s="60"/>
@@ -6961,10 +6904,7 @@
       <c r="I45" s="62"/>
     </row>
     <row r="46" spans="1:9" s="48" customFormat="1" ht="14.25">
-      <c r="A46" s="62">
-        <f t="shared" ca="1" si="1"/>
-        <v>27</v>
-      </c>
+      <c r="A46" s="62"/>
       <c r="B46" s="52"/>
       <c r="C46" s="52"/>
       <c r="D46" s="53"/>
@@ -6975,10 +6915,7 @@
       <c r="I46" s="62"/>
     </row>
     <row r="47" spans="1:9" s="48" customFormat="1" ht="14.25">
-      <c r="A47" s="62">
-        <f t="shared" ca="1" si="1"/>
-        <v>28</v>
-      </c>
+      <c r="A47" s="62"/>
       <c r="B47" s="52"/>
       <c r="C47" s="52"/>
       <c r="D47" s="60"/>
@@ -6989,10 +6926,7 @@
       <c r="I47" s="62"/>
     </row>
     <row r="48" spans="1:9" s="48" customFormat="1" ht="14.25">
-      <c r="A48" s="62">
-        <f t="shared" ca="1" si="1"/>
-        <v>29</v>
-      </c>
+      <c r="A48" s="62"/>
       <c r="B48" s="52"/>
       <c r="C48" s="52"/>
       <c r="D48" s="60"/>
@@ -7003,10 +6937,7 @@
       <c r="I48" s="62"/>
     </row>
     <row r="49" spans="1:9" s="48" customFormat="1" ht="14.25">
-      <c r="A49" s="62">
-        <f t="shared" ca="1" si="1"/>
-        <v>30</v>
-      </c>
+      <c r="A49" s="62"/>
       <c r="B49" s="52"/>
       <c r="C49" s="52"/>
       <c r="D49" s="60"/>
@@ -7017,10 +6948,7 @@
       <c r="I49" s="62"/>
     </row>
     <row r="50" spans="1:9" s="48" customFormat="1" ht="14.25">
-      <c r="A50" s="62">
-        <f t="shared" ca="1" si="1"/>
-        <v>31</v>
-      </c>
+      <c r="A50" s="62"/>
       <c r="B50" s="52"/>
       <c r="C50" s="52"/>
       <c r="D50" s="60"/>
@@ -7032,6 +6960,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
     <mergeCell ref="F16:H16"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="E2:E3"/>
@@ -7039,11 +6972,6 @@
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B18:D18"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation showDropDown="1" showErrorMessage="1" sqref="F16:H17"/>
@@ -7081,10 +7009,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="1" customFormat="1" ht="14.25">
-      <c r="A1" s="193"/>
-      <c r="B1" s="193"/>
-      <c r="C1" s="193"/>
-      <c r="D1" s="193"/>
+      <c r="A1" s="201"/>
+      <c r="B1" s="201"/>
+      <c r="C1" s="201"/>
+      <c r="D1" s="201"/>
       <c r="E1" s="34"/>
       <c r="F1" s="34"/>
       <c r="G1" s="34"/>
@@ -7093,13 +7021,13 @@
       <c r="J1" s="34"/>
     </row>
     <row r="2" spans="1:24" s="1" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A2" s="194" t="s">
+      <c r="A2" s="202" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="194"/>
-      <c r="C2" s="194"/>
-      <c r="D2" s="194"/>
-      <c r="E2" s="202"/>
+      <c r="B2" s="202"/>
+      <c r="C2" s="202"/>
+      <c r="D2" s="202"/>
+      <c r="E2" s="197"/>
       <c r="F2" s="23"/>
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
@@ -7110,7 +7038,7 @@
       <c r="A3" s="47"/>
       <c r="C3" s="204"/>
       <c r="D3" s="204"/>
-      <c r="E3" s="202"/>
+      <c r="E3" s="197"/>
       <c r="F3" s="23"/>
       <c r="G3" s="23"/>
       <c r="H3" s="23"/>
@@ -7121,11 +7049,11 @@
       <c r="A4" s="139" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="196" t="s">
+      <c r="B4" s="199" t="s">
         <v>330</v>
       </c>
-      <c r="C4" s="196"/>
-      <c r="D4" s="196"/>
+      <c r="C4" s="199"/>
+      <c r="D4" s="199"/>
       <c r="E4" s="39"/>
       <c r="F4" s="39"/>
       <c r="G4" s="39"/>
@@ -7139,11 +7067,11 @@
       <c r="A5" s="139" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="195" t="s">
+      <c r="B5" s="200" t="s">
         <v>94</v>
       </c>
-      <c r="C5" s="196"/>
-      <c r="D5" s="196"/>
+      <c r="C5" s="199"/>
+      <c r="D5" s="199"/>
       <c r="E5" s="39"/>
       <c r="F5" s="39"/>
       <c r="G5" s="39"/>
@@ -7157,11 +7085,11 @@
       <c r="A6" s="139" t="s">
         <v>96</v>
       </c>
-      <c r="B6" s="195" t="s">
+      <c r="B6" s="200" t="s">
         <v>97</v>
       </c>
-      <c r="C6" s="196"/>
-      <c r="D6" s="196"/>
+      <c r="C6" s="199"/>
+      <c r="D6" s="199"/>
       <c r="E6" s="39"/>
       <c r="F6" s="39"/>
       <c r="G6" s="39"/>
@@ -7172,11 +7100,11 @@
       <c r="A7" s="139" t="s">
         <v>98</v>
       </c>
-      <c r="B7" s="196" t="s">
+      <c r="B7" s="199" t="s">
         <v>99</v>
       </c>
-      <c r="C7" s="196"/>
-      <c r="D7" s="196"/>
+      <c r="C7" s="199"/>
+      <c r="D7" s="199"/>
       <c r="E7" s="39"/>
       <c r="F7" s="39"/>
       <c r="G7" s="39"/>
@@ -7188,11 +7116,11 @@
       <c r="A8" s="139" t="s">
         <v>100</v>
       </c>
-      <c r="B8" s="197">
+      <c r="B8" s="203">
         <v>40850</v>
       </c>
-      <c r="C8" s="197"/>
-      <c r="D8" s="197"/>
+      <c r="C8" s="203"/>
+      <c r="D8" s="203"/>
       <c r="E8" s="39"/>
     </row>
     <row r="9" spans="1:24" s="43" customFormat="1">
@@ -7373,11 +7301,11 @@
     </row>
     <row r="18" spans="1:9" s="44" customFormat="1" ht="15.75" customHeight="1">
       <c r="A18" s="67"/>
-      <c r="B18" s="201" t="s">
+      <c r="B18" s="208" t="s">
         <v>114</v>
       </c>
-      <c r="C18" s="199"/>
-      <c r="D18" s="200"/>
+      <c r="C18" s="209"/>
+      <c r="D18" s="210"/>
       <c r="E18" s="67"/>
       <c r="F18" s="68"/>
       <c r="G18" s="68"/>
@@ -7656,11 +7584,11 @@
     </row>
     <row r="29" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A29" s="77"/>
-      <c r="B29" s="201" t="s">
+      <c r="B29" s="208" t="s">
         <v>154</v>
       </c>
-      <c r="C29" s="199"/>
-      <c r="D29" s="200"/>
+      <c r="C29" s="209"/>
+      <c r="D29" s="210"/>
       <c r="E29" s="69"/>
       <c r="F29" s="66"/>
       <c r="G29" s="66"/>
@@ -7809,11 +7737,11 @@
     </row>
     <row r="35" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A35" s="77"/>
-      <c r="B35" s="201" t="s">
+      <c r="B35" s="208" t="s">
         <v>173</v>
       </c>
-      <c r="C35" s="199"/>
-      <c r="D35" s="200"/>
+      <c r="C35" s="209"/>
+      <c r="D35" s="210"/>
       <c r="E35" s="69"/>
       <c r="F35" s="66"/>
       <c r="G35" s="66"/>
@@ -7850,11 +7778,11 @@
     </row>
     <row r="37" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A37" s="77"/>
-      <c r="B37" s="201" t="s">
+      <c r="B37" s="208" t="s">
         <v>177</v>
       </c>
-      <c r="C37" s="199"/>
-      <c r="D37" s="200"/>
+      <c r="C37" s="209"/>
+      <c r="D37" s="210"/>
       <c r="E37" s="69"/>
       <c r="F37" s="66"/>
       <c r="G37" s="66"/>
@@ -8115,11 +8043,11 @@
     </row>
     <row r="47" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A47" s="77"/>
-      <c r="B47" s="201" t="s">
+      <c r="B47" s="208" t="s">
         <v>213</v>
       </c>
-      <c r="C47" s="199"/>
-      <c r="D47" s="200"/>
+      <c r="C47" s="209"/>
+      <c r="D47" s="210"/>
       <c r="E47" s="69"/>
       <c r="F47" s="66"/>
       <c r="G47" s="66"/>
@@ -8240,11 +8168,11 @@
     </row>
     <row r="52" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A52" s="77"/>
-      <c r="B52" s="201" t="s">
+      <c r="B52" s="208" t="s">
         <v>228</v>
       </c>
-      <c r="C52" s="199"/>
-      <c r="D52" s="200"/>
+      <c r="C52" s="209"/>
+      <c r="D52" s="210"/>
       <c r="E52" s="69"/>
       <c r="F52" s="66"/>
       <c r="G52" s="66"/>
@@ -8337,11 +8265,11 @@
     </row>
     <row r="56" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A56" s="77"/>
-      <c r="B56" s="201" t="s">
+      <c r="B56" s="208" t="s">
         <v>240</v>
       </c>
-      <c r="C56" s="199"/>
-      <c r="D56" s="200"/>
+      <c r="C56" s="209"/>
+      <c r="D56" s="210"/>
       <c r="E56" s="69"/>
       <c r="F56" s="66"/>
       <c r="G56" s="66"/>
@@ -8658,11 +8586,11 @@
     </row>
     <row r="68" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A68" s="77"/>
-      <c r="B68" s="201" t="s">
+      <c r="B68" s="208" t="s">
         <v>282</v>
       </c>
-      <c r="C68" s="199"/>
-      <c r="D68" s="200"/>
+      <c r="C68" s="209"/>
+      <c r="D68" s="210"/>
       <c r="E68" s="69"/>
       <c r="F68" s="66"/>
       <c r="G68" s="66"/>
@@ -8755,11 +8683,11 @@
     </row>
     <row r="72" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A72" s="77"/>
-      <c r="B72" s="201" t="s">
+      <c r="B72" s="208" t="s">
         <v>292</v>
       </c>
-      <c r="C72" s="199"/>
-      <c r="D72" s="200"/>
+      <c r="C72" s="209"/>
+      <c r="D72" s="210"/>
       <c r="E72" s="69"/>
       <c r="F72" s="66"/>
       <c r="G72" s="66"/>
@@ -8852,11 +8780,11 @@
     </row>
     <row r="76" spans="1:9" s="48" customFormat="1" ht="14.25" customHeight="1">
       <c r="A76" s="77"/>
-      <c r="B76" s="201" t="s">
+      <c r="B76" s="208" t="s">
         <v>303</v>
       </c>
-      <c r="C76" s="199"/>
-      <c r="D76" s="200"/>
+      <c r="C76" s="209"/>
+      <c r="D76" s="210"/>
       <c r="E76" s="69"/>
       <c r="F76" s="66"/>
       <c r="G76" s="66"/>
@@ -8921,11 +8849,11 @@
     </row>
     <row r="79" spans="1:9" s="48" customFormat="1" ht="14.25" customHeight="1">
       <c r="A79" s="77"/>
-      <c r="B79" s="201" t="s">
+      <c r="B79" s="208" t="s">
         <v>311</v>
       </c>
-      <c r="C79" s="199"/>
-      <c r="D79" s="200"/>
+      <c r="C79" s="209"/>
+      <c r="D79" s="210"/>
       <c r="E79" s="69"/>
       <c r="F79" s="66"/>
       <c r="G79" s="66"/>
@@ -9074,17 +9002,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="B72:D72"/>
     <mergeCell ref="B76:D76"/>
@@ -9095,6 +9012,17 @@
     <mergeCell ref="B52:D52"/>
     <mergeCell ref="B56:D56"/>
     <mergeCell ref="B68:D68"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F85:H142">
@@ -9132,10 +9060,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="1" customFormat="1" ht="14.25">
-      <c r="A1" s="193"/>
-      <c r="B1" s="193"/>
-      <c r="C1" s="193"/>
-      <c r="D1" s="193"/>
+      <c r="A1" s="201"/>
+      <c r="B1" s="201"/>
+      <c r="C1" s="201"/>
+      <c r="D1" s="201"/>
       <c r="E1" s="34"/>
       <c r="F1" s="34"/>
       <c r="G1" s="34"/>
@@ -9144,13 +9072,13 @@
       <c r="J1" s="34"/>
     </row>
     <row r="2" spans="1:24" s="1" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A2" s="194" t="s">
+      <c r="A2" s="202" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="194"/>
-      <c r="C2" s="194"/>
-      <c r="D2" s="194"/>
-      <c r="E2" s="202"/>
+      <c r="B2" s="202"/>
+      <c r="C2" s="202"/>
+      <c r="D2" s="202"/>
+      <c r="E2" s="197"/>
       <c r="F2" s="23"/>
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
@@ -9161,7 +9089,7 @@
       <c r="A3" s="47"/>
       <c r="C3" s="204"/>
       <c r="D3" s="204"/>
-      <c r="E3" s="202"/>
+      <c r="E3" s="197"/>
       <c r="F3" s="23"/>
       <c r="G3" s="23"/>
       <c r="H3" s="23"/>
@@ -9172,11 +9100,11 @@
       <c r="A4" s="139" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="196" t="s">
+      <c r="B4" s="199" t="s">
         <v>330</v>
       </c>
-      <c r="C4" s="196"/>
-      <c r="D4" s="196"/>
+      <c r="C4" s="199"/>
+      <c r="D4" s="199"/>
       <c r="E4" s="39"/>
       <c r="F4" s="39"/>
       <c r="G4" s="39"/>
@@ -9190,11 +9118,11 @@
       <c r="A5" s="139" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="195" t="s">
+      <c r="B5" s="200" t="s">
         <v>94</v>
       </c>
-      <c r="C5" s="196"/>
-      <c r="D5" s="196"/>
+      <c r="C5" s="199"/>
+      <c r="D5" s="199"/>
       <c r="E5" s="39"/>
       <c r="F5" s="39"/>
       <c r="G5" s="39"/>
@@ -9208,11 +9136,11 @@
       <c r="A6" s="139" t="s">
         <v>96</v>
       </c>
-      <c r="B6" s="195" t="s">
+      <c r="B6" s="200" t="s">
         <v>97</v>
       </c>
-      <c r="C6" s="196"/>
-      <c r="D6" s="196"/>
+      <c r="C6" s="199"/>
+      <c r="D6" s="199"/>
       <c r="E6" s="39"/>
       <c r="F6" s="39"/>
       <c r="G6" s="39"/>
@@ -9223,11 +9151,11 @@
       <c r="A7" s="139" t="s">
         <v>98</v>
       </c>
-      <c r="B7" s="196" t="s">
+      <c r="B7" s="199" t="s">
         <v>99</v>
       </c>
-      <c r="C7" s="196"/>
-      <c r="D7" s="196"/>
+      <c r="C7" s="199"/>
+      <c r="D7" s="199"/>
       <c r="E7" s="39"/>
       <c r="F7" s="39"/>
       <c r="G7" s="39"/>
@@ -9239,11 +9167,11 @@
       <c r="A8" s="139" t="s">
         <v>100</v>
       </c>
-      <c r="B8" s="197">
+      <c r="B8" s="203">
         <v>40850</v>
       </c>
-      <c r="C8" s="197"/>
-      <c r="D8" s="197"/>
+      <c r="C8" s="203"/>
+      <c r="D8" s="203"/>
       <c r="E8" s="39"/>
     </row>
     <row r="9" spans="1:24" s="43" customFormat="1">
@@ -9424,11 +9352,11 @@
     </row>
     <row r="18" spans="1:9" s="44" customFormat="1" ht="15.75" customHeight="1">
       <c r="A18" s="67"/>
-      <c r="B18" s="201" t="s">
+      <c r="B18" s="208" t="s">
         <v>114</v>
       </c>
-      <c r="C18" s="199"/>
-      <c r="D18" s="200"/>
+      <c r="C18" s="209"/>
+      <c r="D18" s="210"/>
       <c r="E18" s="67"/>
       <c r="F18" s="68"/>
       <c r="G18" s="68"/>
@@ -9709,11 +9637,11 @@
     </row>
     <row r="29" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A29" s="77"/>
-      <c r="B29" s="201" t="s">
+      <c r="B29" s="208" t="s">
         <v>154</v>
       </c>
-      <c r="C29" s="199"/>
-      <c r="D29" s="200"/>
+      <c r="C29" s="209"/>
+      <c r="D29" s="210"/>
       <c r="E29" s="69"/>
       <c r="F29" s="66"/>
       <c r="G29" s="66"/>
@@ -9862,11 +9790,11 @@
     </row>
     <row r="35" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A35" s="77"/>
-      <c r="B35" s="201" t="s">
+      <c r="B35" s="208" t="s">
         <v>173</v>
       </c>
-      <c r="C35" s="199"/>
-      <c r="D35" s="200"/>
+      <c r="C35" s="209"/>
+      <c r="D35" s="210"/>
       <c r="E35" s="69"/>
       <c r="F35" s="66"/>
       <c r="G35" s="66"/>
@@ -9903,11 +9831,11 @@
     </row>
     <row r="37" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A37" s="77"/>
-      <c r="B37" s="201" t="s">
+      <c r="B37" s="208" t="s">
         <v>177</v>
       </c>
-      <c r="C37" s="199"/>
-      <c r="D37" s="200"/>
+      <c r="C37" s="209"/>
+      <c r="D37" s="210"/>
       <c r="E37" s="69"/>
       <c r="F37" s="66"/>
       <c r="G37" s="66"/>
@@ -10168,11 +10096,11 @@
     </row>
     <row r="47" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A47" s="77"/>
-      <c r="B47" s="201" t="s">
+      <c r="B47" s="208" t="s">
         <v>213</v>
       </c>
-      <c r="C47" s="199"/>
-      <c r="D47" s="200"/>
+      <c r="C47" s="209"/>
+      <c r="D47" s="210"/>
       <c r="E47" s="69"/>
       <c r="F47" s="66"/>
       <c r="G47" s="66"/>
@@ -10293,11 +10221,11 @@
     </row>
     <row r="52" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A52" s="77"/>
-      <c r="B52" s="201" t="s">
+      <c r="B52" s="208" t="s">
         <v>228</v>
       </c>
-      <c r="C52" s="199"/>
-      <c r="D52" s="200"/>
+      <c r="C52" s="209"/>
+      <c r="D52" s="210"/>
       <c r="E52" s="69"/>
       <c r="F52" s="66"/>
       <c r="G52" s="66"/>
@@ -10390,11 +10318,11 @@
     </row>
     <row r="56" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A56" s="77"/>
-      <c r="B56" s="201" t="s">
+      <c r="B56" s="208" t="s">
         <v>240</v>
       </c>
-      <c r="C56" s="199"/>
-      <c r="D56" s="200"/>
+      <c r="C56" s="209"/>
+      <c r="D56" s="210"/>
       <c r="E56" s="69"/>
       <c r="F56" s="66"/>
       <c r="G56" s="66"/>
@@ -10711,11 +10639,11 @@
     </row>
     <row r="68" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A68" s="77"/>
-      <c r="B68" s="201" t="s">
+      <c r="B68" s="208" t="s">
         <v>282</v>
       </c>
-      <c r="C68" s="199"/>
-      <c r="D68" s="200"/>
+      <c r="C68" s="209"/>
+      <c r="D68" s="210"/>
       <c r="E68" s="69"/>
       <c r="F68" s="66"/>
       <c r="G68" s="66"/>
@@ -10808,11 +10736,11 @@
     </row>
     <row r="72" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A72" s="77"/>
-      <c r="B72" s="201" t="s">
+      <c r="B72" s="208" t="s">
         <v>292</v>
       </c>
-      <c r="C72" s="199"/>
-      <c r="D72" s="200"/>
+      <c r="C72" s="209"/>
+      <c r="D72" s="210"/>
       <c r="E72" s="69"/>
       <c r="F72" s="66"/>
       <c r="G72" s="66"/>
@@ -10905,11 +10833,11 @@
     </row>
     <row r="76" spans="1:9" s="48" customFormat="1" ht="14.25" customHeight="1">
       <c r="A76" s="77"/>
-      <c r="B76" s="201" t="s">
+      <c r="B76" s="208" t="s">
         <v>303</v>
       </c>
-      <c r="C76" s="199"/>
-      <c r="D76" s="200"/>
+      <c r="C76" s="209"/>
+      <c r="D76" s="210"/>
       <c r="E76" s="69"/>
       <c r="F76" s="66"/>
       <c r="G76" s="66"/>
@@ -10974,11 +10902,11 @@
     </row>
     <row r="79" spans="1:9" s="48" customFormat="1" ht="14.25" customHeight="1">
       <c r="A79" s="77"/>
-      <c r="B79" s="201" t="s">
+      <c r="B79" s="208" t="s">
         <v>311</v>
       </c>
-      <c r="C79" s="199"/>
-      <c r="D79" s="200"/>
+      <c r="C79" s="209"/>
+      <c r="D79" s="210"/>
       <c r="E79" s="69"/>
       <c r="F79" s="66"/>
       <c r="G79" s="66"/>
@@ -11127,6 +11055,17 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="B72:D72"/>
     <mergeCell ref="B76:D76"/>
@@ -11137,17 +11076,6 @@
     <mergeCell ref="B52:D52"/>
     <mergeCell ref="B56:D56"/>
     <mergeCell ref="B68:D68"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B4:D4"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" sqref="F19:H84">
@@ -11204,13 +11132,13 @@
     </row>
     <row r="2" spans="1:12" s="84" customFormat="1" ht="26.25">
       <c r="A2" s="83"/>
-      <c r="C2" s="210" t="s">
+      <c r="C2" s="229" t="s">
         <v>333</v>
       </c>
-      <c r="D2" s="210"/>
-      <c r="E2" s="210"/>
-      <c r="F2" s="210"/>
-      <c r="G2" s="210"/>
+      <c r="D2" s="229"/>
+      <c r="E2" s="229"/>
+      <c r="F2" s="229"/>
+      <c r="G2" s="229"/>
       <c r="H2" s="85" t="s">
         <v>334</v>
       </c>
@@ -11221,15 +11149,15 @@
     </row>
     <row r="3" spans="1:12" s="84" customFormat="1" ht="23.25">
       <c r="A3" s="83"/>
-      <c r="C3" s="211" t="s">
+      <c r="C3" s="230" t="s">
         <v>335</v>
       </c>
-      <c r="D3" s="211"/>
+      <c r="D3" s="230"/>
       <c r="E3" s="157"/>
-      <c r="F3" s="212" t="s">
+      <c r="F3" s="231" t="s">
         <v>336</v>
       </c>
-      <c r="G3" s="212"/>
+      <c r="G3" s="231"/>
       <c r="H3" s="86"/>
       <c r="I3" s="86"/>
       <c r="J3" s="87"/>
@@ -11656,10 +11584,10 @@
       <c r="F26" s="160" t="s">
         <v>384</v>
       </c>
-      <c r="G26" s="214" t="s">
+      <c r="G26" s="232" t="s">
         <v>113</v>
       </c>
-      <c r="H26" s="215"/>
+      <c r="H26" s="233"/>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="100">
@@ -11684,8 +11612,8 @@
         <f>COUNTIFS(#REF!, "*Critical*",#REF!,"*Closed*") + COUNTIFS(#REF!, "*Critical*",#REF!,"*Ready for client test*")</f>
         <v>#REF!</v>
       </c>
-      <c r="G27" s="208"/>
-      <c r="H27" s="209"/>
+      <c r="G27" s="224"/>
+      <c r="H27" s="225"/>
     </row>
     <row r="28" spans="1:12" ht="20.25" customHeight="1">
       <c r="A28" s="100">
@@ -11710,8 +11638,8 @@
         <f>COUNTIFS(#REF!, "*Major*",#REF!,"*Closed*") + COUNTIFS(#REF!, "*Major*",#REF!,"*Ready for client test*")</f>
         <v>#REF!</v>
       </c>
-      <c r="G28" s="208"/>
-      <c r="H28" s="209"/>
+      <c r="G28" s="224"/>
+      <c r="H28" s="225"/>
     </row>
     <row r="29" spans="1:12" ht="20.25" customHeight="1">
       <c r="A29" s="100">
@@ -11736,8 +11664,8 @@
         <f>COUNTIFS(#REF!, "*Normal*",#REF!,"*Closed*") + COUNTIFS(#REF!, "*Normal*",#REF!,"*Ready for client test*")</f>
         <v>#REF!</v>
       </c>
-      <c r="G29" s="208"/>
-      <c r="H29" s="209"/>
+      <c r="G29" s="224"/>
+      <c r="H29" s="225"/>
     </row>
     <row r="30" spans="1:12" ht="20.25" customHeight="1">
       <c r="A30" s="100">
@@ -11762,8 +11690,8 @@
         <f>COUNTIFS(#REF!, "*Minor*",#REF!,"*Closed*") + COUNTIFS(#REF!, "*Minor*",#REF!,"*Ready for client test*")</f>
         <v>#REF!</v>
       </c>
-      <c r="G30" s="208"/>
-      <c r="H30" s="209"/>
+      <c r="G30" s="224"/>
+      <c r="H30" s="225"/>
     </row>
     <row r="31" spans="1:12" ht="20.25" customHeight="1">
       <c r="A31" s="100"/>
@@ -11784,8 +11712,8 @@
         <f>SUM(F27:F30)</f>
         <v>#REF!</v>
       </c>
-      <c r="G31" s="208"/>
-      <c r="H31" s="209"/>
+      <c r="G31" s="224"/>
+      <c r="H31" s="225"/>
     </row>
     <row r="32" spans="1:12" ht="20.25" customHeight="1">
       <c r="A32" s="106"/>
@@ -11823,10 +11751,10 @@
       <c r="E34" s="160" t="s">
         <v>343</v>
       </c>
-      <c r="F34" s="216" t="s">
+      <c r="F34" s="218" t="s">
         <v>346</v>
       </c>
-      <c r="G34" s="217"/>
+      <c r="G34" s="220"/>
     </row>
     <row r="35" spans="1:12" s="125" customFormat="1">
       <c r="A35" s="121"/>
@@ -11842,8 +11770,8 @@
       <c r="E35" s="126" t="s">
         <v>351</v>
       </c>
-      <c r="F35" s="219"/>
-      <c r="G35" s="220"/>
+      <c r="F35" s="227"/>
+      <c r="G35" s="228"/>
       <c r="H35" s="124"/>
       <c r="I35" s="124"/>
       <c r="J35" s="124"/>
@@ -11866,8 +11794,8 @@
       <c r="E36" s="104" t="s">
         <v>357</v>
       </c>
-      <c r="F36" s="208"/>
-      <c r="G36" s="209"/>
+      <c r="F36" s="224"/>
+      <c r="G36" s="225"/>
     </row>
     <row r="37" spans="1:12" ht="20.25" customHeight="1">
       <c r="A37" s="100">
@@ -11885,8 +11813,8 @@
       <c r="E37" s="104" t="s">
         <v>357</v>
       </c>
-      <c r="F37" s="208"/>
-      <c r="G37" s="209"/>
+      <c r="F37" s="224"/>
+      <c r="G37" s="225"/>
     </row>
     <row r="38" spans="1:12" ht="20.25" customHeight="1">
       <c r="A38" s="106"/>
@@ -11926,15 +11854,15 @@
       <c r="B41" s="160" t="s">
         <v>62</v>
       </c>
-      <c r="C41" s="218" t="s">
+      <c r="C41" s="226" t="s">
         <v>400</v>
       </c>
-      <c r="D41" s="218"/>
-      <c r="E41" s="218" t="s">
+      <c r="D41" s="226"/>
+      <c r="E41" s="226" t="s">
         <v>401</v>
       </c>
-      <c r="F41" s="218"/>
-      <c r="G41" s="218"/>
+      <c r="F41" s="226"/>
+      <c r="G41" s="226"/>
       <c r="H41" s="99" t="s">
         <v>402</v>
       </c>
@@ -11946,15 +11874,15 @@
       <c r="B42" s="161" t="s">
         <v>403</v>
       </c>
-      <c r="C42" s="221" t="s">
+      <c r="C42" s="223" t="s">
         <v>404</v>
       </c>
-      <c r="D42" s="221"/>
-      <c r="E42" s="221" t="s">
+      <c r="D42" s="223"/>
+      <c r="E42" s="223" t="s">
         <v>405</v>
       </c>
-      <c r="F42" s="221"/>
-      <c r="G42" s="221"/>
+      <c r="F42" s="223"/>
+      <c r="G42" s="223"/>
       <c r="H42" s="109"/>
     </row>
     <row r="43" spans="1:12" ht="34.5" customHeight="1">
@@ -11964,15 +11892,15 @@
       <c r="B43" s="161" t="s">
         <v>403</v>
       </c>
-      <c r="C43" s="221" t="s">
+      <c r="C43" s="223" t="s">
         <v>404</v>
       </c>
-      <c r="D43" s="221"/>
-      <c r="E43" s="221" t="s">
+      <c r="D43" s="223"/>
+      <c r="E43" s="223" t="s">
         <v>405</v>
       </c>
-      <c r="F43" s="221"/>
-      <c r="G43" s="221"/>
+      <c r="F43" s="223"/>
+      <c r="G43" s="223"/>
       <c r="H43" s="109"/>
     </row>
     <row r="44" spans="1:12" ht="34.5" customHeight="1">
@@ -11982,15 +11910,15 @@
       <c r="B44" s="161" t="s">
         <v>403</v>
       </c>
-      <c r="C44" s="221" t="s">
+      <c r="C44" s="223" t="s">
         <v>404</v>
       </c>
-      <c r="D44" s="221"/>
-      <c r="E44" s="221" t="s">
+      <c r="D44" s="223"/>
+      <c r="E44" s="223" t="s">
         <v>405</v>
       </c>
-      <c r="F44" s="221"/>
-      <c r="G44" s="221"/>
+      <c r="F44" s="223"/>
+      <c r="G44" s="223"/>
       <c r="H44" s="109"/>
     </row>
     <row r="45" spans="1:12">
@@ -12023,25 +11951,25 @@
       <c r="G47" s="98"/>
     </row>
     <row r="48" spans="1:12" s="113" customFormat="1" ht="21" customHeight="1">
-      <c r="A48" s="224" t="s">
+      <c r="A48" s="214" t="s">
         <v>58</v>
       </c>
-      <c r="B48" s="226" t="s">
+      <c r="B48" s="216" t="s">
         <v>408</v>
       </c>
-      <c r="C48" s="216" t="s">
+      <c r="C48" s="218" t="s">
         <v>409</v>
       </c>
-      <c r="D48" s="228"/>
-      <c r="E48" s="228"/>
-      <c r="F48" s="217"/>
-      <c r="G48" s="229" t="s">
+      <c r="D48" s="219"/>
+      <c r="E48" s="219"/>
+      <c r="F48" s="220"/>
+      <c r="G48" s="221" t="s">
         <v>376</v>
       </c>
-      <c r="H48" s="229" t="s">
+      <c r="H48" s="221" t="s">
         <v>408</v>
       </c>
-      <c r="I48" s="222" t="s">
+      <c r="I48" s="211" t="s">
         <v>410</v>
       </c>
       <c r="J48" s="112"/>
@@ -12049,8 +11977,8 @@
       <c r="L48" s="112"/>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="225"/>
-      <c r="B49" s="227"/>
+      <c r="A49" s="215"/>
+      <c r="B49" s="217"/>
       <c r="C49" s="114" t="s">
         <v>385</v>
       </c>
@@ -12063,13 +11991,13 @@
       <c r="F49" s="115" t="s">
         <v>388</v>
       </c>
-      <c r="G49" s="230"/>
-      <c r="H49" s="230"/>
-      <c r="I49" s="223"/>
+      <c r="G49" s="222"/>
+      <c r="H49" s="222"/>
+      <c r="I49" s="212"/>
     </row>
     <row r="50" spans="1:9" ht="38.25">
-      <c r="A50" s="225"/>
-      <c r="B50" s="227"/>
+      <c r="A50" s="215"/>
+      <c r="B50" s="217"/>
       <c r="C50" s="128" t="s">
         <v>411</v>
       </c>
@@ -12181,26 +12109,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="I48:I49"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="C48:F48"/>
-    <mergeCell ref="G48:G49"/>
-    <mergeCell ref="H48:H49"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="F35:G35"/>
     <mergeCell ref="G31:H31"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="C3:D3"/>
@@ -12213,6 +12121,26 @@
     <mergeCell ref="G28:H28"/>
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="G30:H30"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="I48:I49"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="C48:F48"/>
+    <mergeCell ref="G48:G49"/>
+    <mergeCell ref="H48:H49"/>
   </mergeCells>
   <conditionalFormatting sqref="H51">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
@@ -12250,21 +12178,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008DD9373D9A24F64F89F14F461305A106" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="edefd2bea9a69e65a3918d4b9d850884">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cabca498-5e2a-459c-ade0-601c6a98c846" xmlns:ns3="044e8ed5-b60c-40cd-b477-04c240ccf9c3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1cdcf90a8e7cb27405451b504492cec2" ns2:_="" ns3:_="">
     <xsd:import namespace="cabca498-5e2a-459c-ade0-601c6a98c846"/>
@@ -12429,24 +12342,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F8C6C6D-E626-49D4-9BA8-E27B2B9C9191}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06E3E4FA-795A-4742-A021-9CDC3210C50B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7729ACD-7A20-4344-BFA5-B224A8419F45}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12463,4 +12374,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06E3E4FA-795A-4742-A021-9CDC3210C50B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F8C6C6D-E626-49D4-9BA8-E27B2B9C9191}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update notes + relocate files
</commit_message>
<xml_diff>
--- a/Assignment5/TestDesign/TestDesign-Assignment5-QuynhAnh.xlsx
+++ b/Assignment5/TestDesign/TestDesign-Assignment5-QuynhAnh.xlsx
@@ -2750,9 +2750,6 @@
     <t>Check Delete Address function</t>
   </si>
   <si>
-    <t>Delete button is clickable</t>
-  </si>
-  <si>
     <t>- Confirmation pop-up is displayed
 - Confirmation pop-up contains:
 + Alert: "Are you sure you want to delete this address?"
@@ -2799,6 +2796,9 @@
   </si>
   <si>
     <t>Delete successfully if selected address is not default</t>
+  </si>
+  <si>
+    <t>Delete icon is clickable</t>
   </si>
 </sst>
 </file>
@@ -6246,8 +6246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -6579,13 +6579,13 @@
         <v>1</v>
       </c>
       <c r="B20" s="52" t="s">
+        <v>424</v>
+      </c>
+      <c r="C20" s="52" t="s">
         <v>425</v>
       </c>
-      <c r="C20" s="52" t="s">
-        <v>426</v>
-      </c>
       <c r="D20" s="53" t="s">
-        <v>423</v>
+        <v>436</v>
       </c>
       <c r="E20" s="54"/>
       <c r="F20" s="52"/>
@@ -6599,13 +6599,13 @@
         <v>2</v>
       </c>
       <c r="B21" s="52" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C21" s="52" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E21" s="54"/>
       <c r="F21" s="52"/>
@@ -6619,13 +6619,13 @@
         <v>3</v>
       </c>
       <c r="B22" s="52" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C22" s="52" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D22" s="60" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E22" s="52"/>
       <c r="F22" s="52"/>
@@ -6639,7 +6639,7 @@
         <v>4</v>
       </c>
       <c r="B23" s="52" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C23" s="52"/>
       <c r="D23" s="54"/>
@@ -6655,7 +6655,7 @@
         <v>5</v>
       </c>
       <c r="B24" s="52" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C24" s="52"/>
       <c r="D24" s="54"/>
@@ -6671,7 +6671,7 @@
         <v>6</v>
       </c>
       <c r="B25" s="52" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C25" s="52"/>
       <c r="D25" s="54"/>
@@ -6687,7 +6687,7 @@
         <v>7</v>
       </c>
       <c r="B26" s="52" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C26" s="52"/>
       <c r="D26" s="54"/>
@@ -6703,7 +6703,7 @@
         <v>8</v>
       </c>
       <c r="B27" s="52" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C27" s="52"/>
       <c r="D27" s="60"/>

</xml_diff>